<commit_message>
Updated comments for the defect worked.
</commit_message>
<xml_diff>
--- a/docs/QA/Issue tracker_Updated 18_12.xlsx
+++ b/docs/QA/Issue tracker_Updated 18_12.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="468" windowWidth="14808" windowHeight="7656" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Technogy" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="304">
   <si>
     <t>Issue</t>
   </si>
@@ -2577,6 +2577,15 @@
       </rPr>
       <t>put it in the obsevations list</t>
     </r>
+  </si>
+  <si>
+    <t>url have /en/us hence they are not migrated and expcting the same image should exists in chard.</t>
+  </si>
+  <si>
+    <t>suryakanth</t>
+  </si>
+  <si>
+    <t>image is migrated propertly. Issue is with the component rendition, the image is being rendered with the content path instead of image path. OOTB functinlaity</t>
   </si>
 </sst>
 </file>
@@ -2806,14 +2815,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2836,6 +2845,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2844,9 +2856,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2858,6 +2867,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2906,7 +2918,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2941,7 +2953,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3157,20 +3169,20 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="51" style="3" customWidth="1"/>
-    <col min="3" max="3" width="51.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="50.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.109375" style="3"/>
-    <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="3"/>
+    <col min="3" max="3" width="51.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3225,7 +3237,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>79</v>
       </c>
@@ -3280,7 +3292,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>81</v>
       </c>
@@ -3306,7 +3318,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>82</v>
       </c>
@@ -3419,21 +3431,21 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="3"/>
-    <col min="7" max="7" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="3"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3459,7 +3471,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -3488,7 +3500,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
@@ -3514,7 +3526,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>60</v>
       </c>
@@ -3540,7 +3552,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>61</v>
       </c>
@@ -3569,7 +3581,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>62</v>
       </c>
@@ -3595,7 +3607,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -3621,7 +3633,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>64</v>
       </c>
@@ -3647,7 +3659,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>65</v>
       </c>
@@ -3673,7 +3685,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>66</v>
       </c>
@@ -3699,7 +3711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
@@ -3725,11 +3737,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="26" t="s">
         <v>286</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -3748,11 +3760,11 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="26" t="s">
         <v>280</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -3771,7 +3783,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>263</v>
       </c>
@@ -3794,7 +3806,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>264</v>
       </c>
@@ -3817,7 +3829,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="315" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>265</v>
       </c>
@@ -3840,7 +3852,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="24" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="24" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>266</v>
       </c>
@@ -3863,7 +3875,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>267</v>
       </c>
@@ -3886,11 +3898,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="27" t="s">
         <v>275</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -3912,9 +3924,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="26"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="7" t="s">
         <v>257</v>
       </c>
@@ -3974,20 +3986,20 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="51.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="46.88671875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.109375" style="3"/>
-    <col min="8" max="8" width="11.109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="11.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4013,7 +4025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
@@ -4120,7 +4132,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>132</v>
       </c>
@@ -4328,7 +4340,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>197</v>
       </c>
@@ -4354,7 +4366,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>198</v>
       </c>
@@ -4397,16 +4409,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="42.88671875" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
     <col min="4" max="4" width="59" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4432,7 +4444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -4455,7 +4467,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>144</v>
       </c>
@@ -4474,7 +4486,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>145</v>
       </c>
@@ -4497,7 +4509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>146</v>
       </c>
@@ -4520,7 +4532,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>147</v>
       </c>
@@ -4552,20 +4564,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="3"/>
-    <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="57.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="68.33203125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="16.33203125" style="3"/>
+    <col min="1" max="1" width="16.28515625" style="3"/>
+    <col min="2" max="2" width="33.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="68.28515625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="16.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4591,7 +4601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>170</v>
       </c>
@@ -4613,8 +4623,14 @@
       <c r="G2" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="29"/>
       <c r="B3" s="31"/>
       <c r="C3" s="8" t="s">
@@ -4632,8 +4648,14 @@
       <c r="G3" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
       <c r="B4" s="32"/>
       <c r="C4" s="10" t="s">
@@ -4651,8 +4673,14 @@
       <c r="G4" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H4" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>171</v>
       </c>
@@ -4675,7 +4703,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
       <c r="B6" s="33"/>
       <c r="C6" s="8" t="s">
@@ -4694,7 +4722,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="B7" s="33"/>
       <c r="C7" s="10" t="s">
@@ -4713,7 +4741,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="35"/>
       <c r="B8" s="33"/>
       <c r="C8" s="8" t="s">
@@ -4732,7 +4760,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="35"/>
       <c r="B9" s="33"/>
       <c r="C9" s="8" t="s">
@@ -4754,7 +4782,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>172</v>
       </c>
@@ -4776,8 +4804,14 @@
       <c r="G10" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="H10" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>173</v>
       </c>
@@ -4799,12 +4833,18 @@
       <c r="G11" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H11" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="36" t="s">
         <v>99</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -4823,9 +4863,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="28"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="8" t="s">
         <v>90</v>
       </c>
@@ -4842,9 +4882,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="29"/>
-      <c r="B14" s="28"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="8" t="s">
         <v>96</v>
       </c>
@@ -4861,9 +4901,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
-      <c r="B15" s="28"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="10" t="s">
         <v>94</v>
       </c>
@@ -4903,11 +4943,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="36" t="s">
         <v>101</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -4926,9 +4966,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="28"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="10" t="s">
         <v>92</v>
       </c>
@@ -5060,11 +5100,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="36" t="s">
         <v>111</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -5083,9 +5123,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="28"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="10" t="s">
         <v>105</v>
       </c>
@@ -5196,16 +5236,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A24:A25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -5235,18 +5275,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.88671875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="41.109375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="58.33203125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="16"/>
+    <col min="1" max="1" width="8.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.85546875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="58.28515625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5278,7 +5318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>201</v>
       </c>
@@ -5301,11 +5341,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>299</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -5324,9 +5364,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="16" t="s">
         <v>206</v>
       </c>
@@ -5343,9 +5383,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="16" t="s">
         <v>208</v>
       </c>
@@ -5362,8 +5402,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>210</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -5385,8 +5425,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
       <c r="C7" s="16" t="s">
         <v>206</v>
       </c>
@@ -5449,11 +5489,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="38" t="s">
         <v>218</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -5472,9 +5512,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="16" t="s">
         <v>208</v>
       </c>
@@ -5537,7 +5577,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>225</v>
       </c>
@@ -5580,12 +5620,12 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
-    <col min="4" max="4" width="67.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5680,14 +5720,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="16"/>
-    <col min="2" max="2" width="52.109375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="53.6640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="16"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="2" max="2" width="52.140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="53.7109375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5719,11 +5759,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>205</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -5742,9 +5782,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="16" t="s">
         <v>238</v>
       </c>
@@ -5761,9 +5801,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="16" t="s">
         <v>240</v>
       </c>
@@ -5912,11 +5952,11 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="51.5546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code to fix the issue with the dam assets.
</commit_message>
<xml_diff>
--- a/docs/QA/Issue tracker_Updated 18_12.xlsx
+++ b/docs/QA/Issue tracker_Updated 18_12.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="309">
   <si>
     <t>Issue</t>
   </si>
@@ -2586,6 +2586,21 @@
   </si>
   <si>
     <t>image is migrated propertly. Issue is with the component rendition, the image is being rendered with the content path instead of image path. OOTB functinlaity</t>
+  </si>
+  <si>
+    <t>Re-test</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>no code written to migrate the dam. Updated the code.</t>
+  </si>
+  <si>
+    <t>Not an issue since no html blob found on web publisher to migrate.</t>
+  </si>
+  <si>
+    <t>Not an issue since no html blob found on WEM publisher to migrate.</t>
   </si>
 </sst>
 </file>
@@ -2824,6 +2839,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2844,9 +2862,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4602,10 +4617,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>291</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -4618,7 +4633,7 @@
         <v>42355</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>87</v>
@@ -4631,8 +4646,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="8" t="s">
         <v>88</v>
       </c>
@@ -4643,7 +4658,7 @@
         <v>42355</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>87</v>
@@ -4656,8 +4671,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="10" t="s">
         <v>88</v>
       </c>
@@ -4668,7 +4683,7 @@
         <v>42355</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>87</v>
@@ -4681,10 +4696,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>292</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -4704,8 +4719,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="8" t="s">
         <v>90</v>
       </c>
@@ -4723,8 +4738,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="10" t="s">
         <v>92</v>
       </c>
@@ -4742,8 +4757,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="8" t="s">
         <v>94</v>
       </c>
@@ -4761,8 +4776,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="8" t="s">
         <v>96</v>
       </c>
@@ -4799,7 +4814,7 @@
         <v>42355</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>87</v>
@@ -4828,7 +4843,7 @@
         <v>42355</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>87</v>
@@ -4840,11 +4855,11 @@
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="29" t="s">
         <v>99</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -4857,15 +4872,21 @@
         <v>42355</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>11</v>
+        <v>304</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="36"/>
+      <c r="H12" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="8" t="s">
         <v>90</v>
       </c>
@@ -4876,15 +4897,21 @@
         <v>42355</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>11</v>
+        <v>304</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="36"/>
+      <c r="H13" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="8" t="s">
         <v>96</v>
       </c>
@@ -4895,15 +4922,21 @@
         <v>42355</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>11</v>
+        <v>304</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="36"/>
+      <c r="H14" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="10" t="s">
         <v>94</v>
       </c>
@@ -4914,10 +4947,16 @@
         <v>42355</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>11</v>
+        <v>304</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>87</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4944,10 +4983,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="29" t="s">
         <v>101</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -4967,8 +5006,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="36"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10" t="s">
         <v>92</v>
       </c>
@@ -5101,10 +5140,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="29" t="s">
         <v>111</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -5124,8 +5163,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="36"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="10" t="s">
         <v>105</v>
       </c>
@@ -5236,16 +5275,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B12:B15"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B12:B15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated comments in the sheet for the defect on dam images.
</commit_message>
<xml_diff>
--- a/docs/QA/Issue tracker_Updated 18_12.xlsx
+++ b/docs/QA/Issue tracker_Updated 18_12.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="311">
   <si>
     <t>Issue</t>
   </si>
@@ -2601,6 +2601,12 @@
   </si>
   <si>
     <t>Not an issue since no html blob found on WEM publisher to migrate.</t>
+  </si>
+  <si>
+    <t>Image are being rendered from css. Need to update css. Tested by updating css file in firebug, working fine.</t>
+  </si>
+  <si>
+    <t>url have /c/dam hence they are not migrated and expcting the same image should exists in chard.</t>
   </si>
 </sst>
 </file>
@@ -4616,7 +4622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>170</v>
       </c>
@@ -4976,20 +4982,26 @@
         <v>42355</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>11</v>
+        <v>304</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H16" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>180</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D17" s="10" t="s">
@@ -4999,13 +5011,19 @@
         <v>42355</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H17" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="B18" s="29"/>
       <c r="C18" s="10" t="s">
@@ -5018,13 +5036,19 @@
         <v>42355</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H18" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>181</v>
       </c>
@@ -5041,13 +5065,19 @@
         <v>42355</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H19" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>182</v>
       </c>
@@ -5069,8 +5099,9 @@
       <c r="G20" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="I20" s="25"/>
+    </row>
+    <row r="21" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>183</v>
       </c>
@@ -5087,13 +5118,19 @@
         <v>42355</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="H21" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>184</v>
       </c>
@@ -5110,13 +5147,19 @@
         <v>42355</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="H22" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>185</v>
       </c>
@@ -5133,20 +5176,26 @@
         <v>42355</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H23" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>186</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>109</v>
       </c>
       <c r="D24" s="10" t="s">
@@ -5156,13 +5205,19 @@
         <v>42355</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H24" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="30"/>
       <c r="B25" s="29"/>
       <c r="C25" s="10" t="s">
@@ -5175,13 +5230,19 @@
         <v>42355</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="H25" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>187</v>
       </c>
@@ -5204,7 +5265,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>188</v>
       </c>
@@ -5227,7 +5288,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>189</v>
       </c>
@@ -5244,13 +5305,19 @@
         <v>42357</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="H28" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>190</v>
       </c>
@@ -5267,10 +5334,16 @@
         <v>42358</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>87</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -5304,9 +5377,11 @@
     <hyperlink ref="D27" r:id="rId15"/>
     <hyperlink ref="C26" r:id="rId16"/>
     <hyperlink ref="D26" r:id="rId17"/>
+    <hyperlink ref="C17" r:id="rId18"/>
+    <hyperlink ref="C24" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated sheet with comment and fix.
</commit_message>
<xml_diff>
--- a/docs/QA/Issue tracker_Updated 18_12.xlsx
+++ b/docs/QA/Issue tracker_Updated 18_12.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Technogy" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="311">
   <si>
     <t>Issue</t>
   </si>
@@ -2767,7 +2767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2822,9 +2822,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2843,10 +2840,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2869,14 +2875,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3762,7 +3771,7 @@
       <c r="A12" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>286</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -3785,7 +3794,7 @@
       <c r="A13" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="25" t="s">
         <v>280</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -3808,7 +3817,7 @@
       <c r="A14" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>279</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -3831,7 +3840,7 @@
       <c r="A15" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>278</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -3854,7 +3863,7 @@
       <c r="A16" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="23" t="s">
         <v>277</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -3873,11 +3882,11 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="24" customFormat="1" ht="300" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+    <row r="17" spans="1:8" s="23" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="24" t="s">
         <v>276</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -3886,13 +3895,13 @@
       <c r="D17" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="24" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3920,10 +3929,10 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="30" t="s">
         <v>275</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -3946,8 +3955,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="27"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="7" t="s">
         <v>257</v>
       </c>
@@ -4585,7 +4594,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4623,10 +4634,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="33" t="s">
         <v>291</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -4652,8 +4663,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="8" t="s">
         <v>88</v>
       </c>
@@ -4672,13 +4683,13 @@
       <c r="H3" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="10" t="s">
         <v>88</v>
       </c>
@@ -4697,15 +4708,15 @@
       <c r="H4" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="36" t="s">
         <v>292</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -4725,8 +4736,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="8" t="s">
         <v>90</v>
       </c>
@@ -4744,8 +4755,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="10" t="s">
         <v>92</v>
       </c>
@@ -4763,8 +4774,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="8" t="s">
         <v>94</v>
       </c>
@@ -4782,8 +4793,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="8" t="s">
         <v>96</v>
       </c>
@@ -4854,18 +4865,18 @@
       <c r="G11" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="24" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="39" t="s">
         <v>99</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -4891,8 +4902,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="8" t="s">
         <v>90</v>
       </c>
@@ -4908,7 +4919,7 @@
       <c r="G13" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="24" t="s">
         <v>302</v>
       </c>
       <c r="I13" s="3" t="s">
@@ -4916,8 +4927,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="8" t="s">
         <v>96</v>
       </c>
@@ -4941,8 +4952,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="10" t="s">
         <v>94</v>
       </c>
@@ -4958,10 +4969,10 @@
       <c r="G15" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="I15" s="24" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4990,15 +5001,15 @@
       <c r="H16" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="24" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="39" t="s">
         <v>101</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -5024,8 +5035,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="10" t="s">
         <v>92</v>
       </c>
@@ -5044,7 +5055,7 @@
       <c r="H18" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="I18" s="24" t="s">
         <v>309</v>
       </c>
     </row>
@@ -5073,7 +5084,7 @@
       <c r="H19" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="I19" s="25" t="s">
+      <c r="I19" s="24" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5099,7 +5110,7 @@
       <c r="G20" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I20" s="25"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -5126,7 +5137,7 @@
       <c r="H21" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="I21" s="25" t="s">
+      <c r="I21" s="24" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5152,10 +5163,10 @@
       <c r="G22" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="I22" s="25" t="s">
+      <c r="I22" s="24" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5181,18 +5192,18 @@
       <c r="G23" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="I23" s="24" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="39" t="s">
         <v>111</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -5210,16 +5221,16 @@
       <c r="G24" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H24" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="I24" s="25" t="s">
+      <c r="I24" s="24" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="29"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="10" t="s">
         <v>105</v>
       </c>
@@ -5235,10 +5246,10 @@
       <c r="G25" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="I25" s="25" t="s">
+      <c r="I25" s="24" t="s">
         <v>309</v>
       </c>
     </row>
@@ -5313,7 +5324,7 @@
       <c r="H28" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="I28" s="25" t="s">
+      <c r="I28" s="24" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5339,25 +5350,25 @@
       <c r="G29" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="25" t="s">
+      <c r="H29" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="I29" s="25" t="s">
+      <c r="I29" s="24" t="s">
         <v>303</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A24:A25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -5389,8 +5400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5400,318 +5411,364 @@
     <col min="3" max="3" width="41.140625" style="16" customWidth="1"/>
     <col min="4" max="4" width="58.28515625" style="16" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="16"/>
+    <col min="6" max="7" width="9.140625" style="16"/>
+    <col min="8" max="8" width="10.5703125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="56.28515625" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="27" t="s">
         <v>295</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="29">
         <v>42356</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="29">
+        <v>42356</v>
+      </c>
+      <c r="F3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G3" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>299</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="29">
         <v>42356</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G4" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="16" t="s">
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="40"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="29">
+        <v>42356</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" s="29">
+        <v>42356</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="40"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D7" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E7" s="29">
         <v>42356</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G7" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="16" t="s">
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" s="29">
+        <v>42356</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="29">
+        <v>42356</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="29">
+        <v>42356</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D11" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E11" s="29">
         <v>42356</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F11" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G11" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="E6" s="4">
-        <v>42356</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="C7" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="E7" s="4">
-        <v>42356</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="E8" s="4">
-        <v>42356</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="E9" s="4">
-        <v>42356</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>218</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="4">
-        <v>42356</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="E11" s="4">
-        <v>42356</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>87</v>
-      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="27" t="s">
         <v>219</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="29">
         <v>42356</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="16" t="s">
+      <c r="F12" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="G12" s="27" t="s">
         <v>87</v>
       </c>
+      <c r="H12" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="27" t="s">
         <v>223</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="29">
         <v>42356</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="G13" s="27" t="s">
         <v>87</v>
       </c>
+      <c r="H13" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="29">
         <v>42356</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="16" t="s">
+      <c r="F14" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="G14" s="27" t="s">
         <v>87</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -5731,7 +5788,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5740,6 +5797,8 @@
     <col min="3" max="3" width="64" customWidth="1"/>
     <col min="4" max="4" width="67.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5803,7 +5862,7 @@
       <c r="B3" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="5" t="s">
         <v>233</v>
       </c>
       <c r="D3" s="16" t="s">
@@ -5813,15 +5872,22 @@
         <v>42356</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>11</v>
+        <v>305</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="H3" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>309</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5830,8 +5896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5841,219 +5907,245 @@
     <col min="3" max="3" width="53.5703125" style="16" customWidth="1"/>
     <col min="4" max="4" width="53.7109375" style="16" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="16"/>
+    <col min="6" max="7" width="9.140625" style="16"/>
+    <col min="8" max="8" width="11.28515625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="27" t="s">
         <v>235</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="29">
         <v>42356</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="27" t="s">
         <v>87</v>
       </c>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="16" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="29">
         <v>42356</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="27" t="s">
         <v>87</v>
       </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="16" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="27" t="s">
         <v>241</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="29">
         <v>42356</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="27" t="s">
         <v>87</v>
       </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="29">
         <v>42356</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="E6" s="29">
+        <v>42356</v>
+      </c>
+      <c r="F6" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G6" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D7" s="27" t="s">
         <v>241</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E7" s="29">
         <v>42356</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F7" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G7" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" s="29">
         <v>42356</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F8" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G8" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="C8" s="16" t="s">
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D9" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E9" s="29">
         <v>42356</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F9" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G9" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="E9" s="4">
-        <v>42356</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>87</v>
-      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated comment to fix the issue with the dam assets.
</commit_message>
<xml_diff>
--- a/docs/QA/Issue tracker_Updated 18_12.xlsx
+++ b/docs/QA/Issue tracker_Updated 18_12.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="311">
   <si>
     <t>Issue</t>
   </si>
@@ -2848,6 +2848,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2883,9 +2886,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3929,10 +3929,10 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>275</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -3955,8 +3955,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="30"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="7" t="s">
         <v>257</v>
       </c>
@@ -4594,8 +4594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4634,10 +4634,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>291</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -4663,8 +4663,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="8" t="s">
         <v>88</v>
       </c>
@@ -4688,8 +4688,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="10" t="s">
         <v>88</v>
       </c>
@@ -4713,10 +4713,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>292</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -4736,8 +4736,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="8" t="s">
         <v>90</v>
       </c>
@@ -4755,8 +4755,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="10" t="s">
         <v>92</v>
       </c>
@@ -4774,8 +4774,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="36"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="8" t="s">
         <v>94</v>
       </c>
@@ -4793,8 +4793,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="8" t="s">
         <v>96</v>
       </c>
@@ -4873,10 +4873,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="40" t="s">
         <v>99</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -4902,8 +4902,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="39"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="8" t="s">
         <v>90</v>
       </c>
@@ -4927,8 +4927,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="39"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="8" t="s">
         <v>96</v>
       </c>
@@ -4952,8 +4952,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="10" t="s">
         <v>94</v>
       </c>
@@ -5006,10 +5006,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="40" t="s">
         <v>101</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -5035,8 +5035,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10" t="s">
         <v>92</v>
       </c>
@@ -5200,10 +5200,10 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="40" t="s">
         <v>111</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -5229,8 +5229,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="39"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="10" t="s">
         <v>105</v>
       </c>
@@ -5400,8 +5400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5476,10 +5476,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>299</v>
       </c>
       <c r="C3" s="27" t="s">
@@ -5501,8 +5501,8 @@
       <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="27" t="s">
         <v>206</v>
       </c>
@@ -5522,8 +5522,8 @@
       <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="27" t="s">
         <v>208</v>
       </c>
@@ -5543,7 +5543,7 @@
       <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>210</v>
       </c>
       <c r="B6" s="27" t="s">
@@ -5568,7 +5568,7 @@
       <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="27"/>
       <c r="C7" s="27" t="s">
         <v>206</v>
@@ -5639,10 +5639,10 @@
       <c r="I9" s="27"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="31" t="s">
         <v>218</v>
       </c>
       <c r="C10" s="27" t="s">
@@ -5664,8 +5664,8 @@
       <c r="I10" s="27"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="27" t="s">
         <v>208</v>
       </c>
@@ -5897,7 +5897,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5943,10 +5943,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>205</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -5968,8 +5968,8 @@
       <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="30"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="27" t="s">
         <v>238</v>
       </c>
@@ -5989,8 +5989,8 @@
       <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="27" t="s">
         <v>240</v>
       </c>
@@ -6016,7 +6016,7 @@
       <c r="B5" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="30" t="s">
         <v>238</v>
       </c>
       <c r="D5" s="27" t="s">
@@ -6080,13 +6080,17 @@
         <v>42356</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>237</v>
+        <v>305</v>
       </c>
       <c r="G7" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
+      <c r="H7" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
@@ -6095,7 +6099,7 @@
       <c r="B8" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="30" t="s">
         <v>247</v>
       </c>
       <c r="D8" s="27" t="s">
@@ -6113,7 +6117,7 @@
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>249</v>
       </c>
@@ -6130,13 +6134,17 @@
         <v>42356</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>237</v>
+        <v>305</v>
       </c>
       <c r="G9" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
+      <c r="H9" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>310</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6145,6 +6153,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>